<commit_message>
Merge - Opp Test Data, ENg Detail, Add Counterparty - 10 Oct 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_T1426_OpportunityToEngagementConversionMappingForCF.xlsx
+++ b/TestData/LV_T1426_OpportunityToEngagementConversionMappingForCF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304A8E7C-8A41-4E26-9EF4-8B805DFEEF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7514941F-C9AD-49A8-9FBA-DF8C8C7AE7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="548" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="548" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StandardUsers" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="AddOpportunity" sheetId="12" r:id="rId5"/>
     <sheet name="AddContact" sheetId="14" r:id="rId6"/>
     <sheet name="Engagement" sheetId="15" r:id="rId7"/>
+    <sheet name="ProductType" sheetId="17" r:id="rId8"/>
+    <sheet name="Notes" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="104">
   <si>
     <t>James Craven</t>
   </si>
@@ -251,9 +253,6 @@
     <t>Lender Education</t>
   </si>
   <si>
-    <t>Capital Markets</t>
-  </si>
-  <si>
     <t>Buyside</t>
   </si>
   <si>
@@ -269,9 +268,6 @@
     <t>Real Estate Brokerage</t>
   </si>
   <si>
-    <t>Special Committee Advisory</t>
-  </si>
-  <si>
     <t>Strategic Alternatives Study</t>
   </si>
   <si>
@@ -281,15 +277,6 @@
     <t>Activism Advisory</t>
   </si>
   <si>
-    <t>Strategy</t>
-  </si>
-  <si>
-    <t>Post Merger Integration</t>
-  </si>
-  <si>
-    <t>Valuation Advisory</t>
-  </si>
-  <si>
     <t>Advisory (CF)</t>
   </si>
   <si>
@@ -302,14 +289,80 @@
     <t>Engagements</t>
   </si>
   <si>
-    <t>Brian Miller</t>
+    <t>Compliance User</t>
+  </si>
+  <si>
+    <t>Lorriane Johnson</t>
+  </si>
+  <si>
+    <t>Legal User</t>
+  </si>
+  <si>
+    <t>Christine Sha</t>
+  </si>
+  <si>
+    <t>Legal Hold test Notes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Jennie Stewart</t>
+  </si>
+  <si>
+    <t>Debt Financing</t>
+  </si>
+  <si>
+    <t>Directs</t>
+  </si>
+  <si>
+    <t>Primary Capital Advisory</t>
+  </si>
+  <si>
+    <t>Capital Solutions</t>
+  </si>
+  <si>
+    <t>Equity Placements</t>
+  </si>
+  <si>
+    <t>GP Stake Sale</t>
+  </si>
+  <si>
+    <t>LP-Led Secondaries</t>
+  </si>
+  <si>
+    <t>Liability Management</t>
+  </si>
+  <si>
+    <t>Advisory</t>
+  </si>
+  <si>
+    <t>ProductType</t>
+  </si>
+  <si>
+    <t>ERPProductTypeCode</t>
+  </si>
+  <si>
+    <t>ADV</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Ajay Nair</t>
+  </si>
+  <si>
+    <t>System Admin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,19 +499,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -660,57 +713,51 @@
   <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyFont="0" applyFill="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyFont="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyFont="0" applyFill="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyFont="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyFont="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" applyFill="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyFont="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="8" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyFont="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyFont="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{18F405CE-23A4-4C4C-B371-AE456DF50166}"/>
@@ -1068,15 +1115,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FBB8EB1-471A-4668-845A-6810E22F6BA4}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1089,10 +1137,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1131,7 +1203,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1223,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1162,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD13242-055E-41A8-80D8-6F50F1B57F7C}">
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1248,7 @@
     <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1259,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -1268,18 +1340,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>78</v>
+      <c r="C2" t="s">
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
@@ -1359,22 +1431,19 @@
       <c r="AD2" t="s">
         <v>55</v>
       </c>
-      <c r="AE2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
       <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>71</v>
+      <c r="C3" t="s">
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -1454,22 +1523,19 @@
       <c r="AD3" t="s">
         <v>55</v>
       </c>
-      <c r="AE3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>68</v>
+      <c r="C4" t="s">
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
         <v>40</v>
@@ -1549,22 +1615,19 @@
       <c r="AD4" t="s">
         <v>55</v>
       </c>
-      <c r="AE4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>70</v>
+      <c r="C5" t="s">
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -1644,22 +1707,19 @@
       <c r="AD5" t="s">
         <v>55</v>
       </c>
-      <c r="AE5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>72</v>
+      <c r="C6" t="s">
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1739,22 +1799,19 @@
       <c r="AD6" t="s">
         <v>55</v>
       </c>
-      <c r="AE6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>73</v>
+      <c r="C7" t="s">
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
@@ -1834,22 +1891,19 @@
       <c r="AD7" t="s">
         <v>55</v>
       </c>
-      <c r="AE7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>74</v>
+      <c r="C8" t="s">
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -1929,22 +1983,19 @@
       <c r="AD8" t="s">
         <v>55</v>
       </c>
-      <c r="AE8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>75</v>
+      <c r="C9" t="s">
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -2024,22 +2075,19 @@
       <c r="AD9" t="s">
         <v>55</v>
       </c>
-      <c r="AE9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>76</v>
+      <c r="C10" t="s">
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -2119,22 +2167,19 @@
       <c r="AD10" t="s">
         <v>55</v>
       </c>
-      <c r="AE10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>77</v>
+      <c r="C11" t="s">
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -2214,22 +2259,19 @@
       <c r="AD11" t="s">
         <v>55</v>
       </c>
-      <c r="AE11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
         <v>79</v>
-      </c>
-      <c r="D12" t="s">
-        <v>84</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -2309,22 +2351,19 @@
       <c r="AD12" t="s">
         <v>55</v>
       </c>
-      <c r="AE12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>80</v>
+      <c r="C13" t="s">
+        <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -2404,22 +2443,19 @@
       <c r="AD13" t="s">
         <v>55</v>
       </c>
-      <c r="AE13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>81</v>
+      <c r="C14" t="s">
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
@@ -2499,8 +2535,281 @@
       <c r="AD14" t="s">
         <v>55</v>
       </c>
-      <c r="AE14">
-        <v>13</v>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R15" t="s">
+        <v>47</v>
+      </c>
+      <c r="S15" t="s">
+        <v>47</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U15" t="s">
+        <v>49</v>
+      </c>
+      <c r="V15" t="s">
+        <v>50</v>
+      </c>
+      <c r="W15" t="s">
+        <v>51</v>
+      </c>
+      <c r="X15" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" t="s">
+        <v>47</v>
+      </c>
+      <c r="S16" t="s">
+        <v>47</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U16" t="s">
+        <v>49</v>
+      </c>
+      <c r="V16" t="s">
+        <v>50</v>
+      </c>
+      <c r="W16" t="s">
+        <v>51</v>
+      </c>
+      <c r="X16" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17" t="s">
+        <v>45</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="R17" t="s">
+        <v>47</v>
+      </c>
+      <c r="S17" t="s">
+        <v>47</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U17" t="s">
+        <v>49</v>
+      </c>
+      <c r="V17" t="s">
+        <v>50</v>
+      </c>
+      <c r="W17" t="s">
+        <v>51</v>
+      </c>
+      <c r="X17" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2515,7 +2824,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2386AE-B180-4489-BA71-14068DFEFD5A}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,10 +2920,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -2622,138 +2931,354 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
         <v>77</v>
       </c>
-      <c r="B11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11">
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17">
         <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF8D60A-1002-4D00-B235-C15EB6546928}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9447574-C5CB-49C4-BC94-993C1D07E71B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>